<commit_message>
New cross validation setup
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B81A73E-D726-48EB-BBC2-218785DA685C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC837595-796B-4B63-B5F6-B62B1C7B4A25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20625" yWindow="6300" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="No-PCA" sheetId="1" r:id="rId1"/>
-    <sheet name="PCA" sheetId="2" r:id="rId2"/>
-    <sheet name="Classifiers" sheetId="3" r:id="rId3"/>
+    <sheet name="Compiled - Combined Data" sheetId="4" r:id="rId1"/>
+    <sheet name="No-PCA" sheetId="1" r:id="rId2"/>
+    <sheet name="PCA" sheetId="2" r:id="rId3"/>
+    <sheet name="Classifiers" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="92">
   <si>
     <t>Type</t>
   </si>
@@ -247,6 +248,57 @@
   </si>
   <si>
     <t>(100, 10)</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Average age difference</t>
+  </si>
+  <si>
+    <t>Average absolute diff</t>
+  </si>
+  <si>
+    <t>Bayesian Ridge</t>
+  </si>
+  <si>
+    <t>SVM - RBF</t>
+  </si>
+  <si>
+    <t>R^2 final</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>R^2 in CV</t>
+  </si>
+  <si>
+    <t>Ridge</t>
+  </si>
+  <si>
+    <t>ElasticNet</t>
+  </si>
+  <si>
+    <t>Lars</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>NN (50)</t>
+  </si>
+  <si>
+    <t>NN (25)</t>
+  </si>
+  <si>
+    <t>NN (10)</t>
+  </si>
+  <si>
+    <t>NN (5)</t>
+  </si>
+  <si>
+    <t>NN (2)</t>
   </si>
 </sst>
 </file>
@@ -282,9 +334,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,10 +617,243 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F02596-180B-41D3-A612-B08F6A794E6B}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="E2">
+        <v>3.5960000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="C3">
+        <v>0.997</v>
+      </c>
+      <c r="D3">
+        <v>-0.48599999999999999</v>
+      </c>
+      <c r="E3">
+        <v>1.4570000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>-3.6469999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="D4">
+        <v>-0.52900000000000003</v>
+      </c>
+      <c r="E4">
+        <v>2.891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5">
+        <v>-0.37</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>-0.69699999999999995</v>
+      </c>
+      <c r="E5">
+        <v>1.9870000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="D6">
+        <v>-0.51800000000000002</v>
+      </c>
+      <c r="E6">
+        <v>3.2589999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="D7">
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="E7">
+        <v>3.266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="C8">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="D8">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="E8">
+        <v>3.9380000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-6.8900000000000004E+34</v>
+      </c>
+      <c r="C9">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="D9">
+        <v>-0.188</v>
+      </c>
+      <c r="E9">
+        <v>8.2620000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="D10">
+        <v>-1.736</v>
+      </c>
+      <c r="E10">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>-0.71099999999999997</v>
+      </c>
+      <c r="E11">
+        <v>2.7370000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
@@ -2044,7 +2330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13511E3B-26B4-4710-BEC4-91093390E4E7}">
   <dimension ref="A1:E61"/>
   <sheetViews>
@@ -2747,11 +3033,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6EBC8-43E5-4815-B776-F59CCADE54BE}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>

</xml_diff>